<commit_message>
RSI fast & slow
</commit_message>
<xml_diff>
--- a/pdfcreater/excel/RSI横截面_纯多头_sh300_日频_每年重置_OUTPUT.xlsx
+++ b/pdfcreater/excel/RSI横截面_纯多头_sh300_日频_每年重置_OUTPUT.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meiconte\Desktop\pdfcreater\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>收益率</t>
   </si>
@@ -36,34 +32,34 @@
     <t>最大回撤发生时间段</t>
   </si>
   <si>
-    <t>2008.02 - 2008.12</t>
-  </si>
-  <si>
-    <t>2008.03.03 - 2008.12.29</t>
+    <t>2008.01 - 2008.12</t>
+  </si>
+  <si>
+    <t>2008.01.14 - 2008.11.12</t>
   </si>
   <si>
     <t>2009.01 - 2009.12</t>
   </si>
   <si>
-    <t>2009.08.04 - 2009.09.30</t>
+    <t>2009.08.04 - 2009.09.03</t>
   </si>
   <si>
     <t>2010.01 - 2010.12</t>
   </si>
   <si>
-    <t>2010.11.08 - 2010.12.29</t>
+    <t>2010.01.18 - 2010.07.19</t>
   </si>
   <si>
     <t>2011.01 - 2011.12</t>
   </si>
   <si>
-    <t>2011.02.21 - 2011.12.29</t>
+    <t>2011.07.18 - 2011.12.30</t>
   </si>
   <si>
     <t>2012.01 - 2012.12</t>
   </si>
   <si>
-    <t>2012.03.13 - 2012.12.14</t>
+    <t>2012.03.02 - 2012.11.30</t>
   </si>
   <si>
     <t>2013.01 - 2013.12</t>
@@ -75,64 +71,54 @@
     <t>2014.01 - 2014.12</t>
   </si>
   <si>
-    <t>2014.02.19 - 2014.06.23</t>
+    <t>2014.12.19 - 2014.12.25</t>
   </si>
   <si>
     <t>2015.01 - 2015.12</t>
   </si>
   <si>
-    <t>2015.06.12 - 2015.11.04</t>
+    <t>2015.06.12 - 2015.09.28</t>
   </si>
   <si>
     <t>2016.01 - 2016.12</t>
   </si>
   <si>
-    <t>2016.01.06 - 2016.05.31</t>
+    <t>2016.02.22 - 2016.06.27</t>
   </si>
   <si>
     <t>2017.01 - 2017.12</t>
   </si>
   <si>
-    <t>2017.08.08 - 2017.08.25</t>
+    <t>2017.11.21 - 2017.12.19</t>
   </si>
   <si>
     <t>2018.01 - 2018.10</t>
   </si>
   <si>
-    <t>2018.01.26 - 2018.10.24</t>
-  </si>
-  <si>
-    <t>HS300收益率</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>2018.01.26 - 2018.10.25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="fangsong"/>
       <sz val="10"/>
-      <name val="fangsong"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -148,42 +134,33 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="00000000"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="00000000"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="00000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="00000000"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="40" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -471,323 +448,284 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="16"/>
+    <col customWidth="1" max="2" min="2" width="12"/>
+    <col customWidth="1" max="3" min="3" width="12"/>
+    <col customWidth="1" max="4" min="4" width="12"/>
+    <col customWidth="1" max="5" min="5" width="12"/>
+    <col customWidth="1" max="6" min="6" width="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2">
-        <v>-9.43704045628595E-2</v>
-      </c>
-      <c r="C2" s="2">
-        <v>-0.66245399999999999</v>
-      </c>
-      <c r="D2" s="2">
-        <v>-9.43704045628595E-2</v>
-      </c>
-      <c r="E2" s="2">
-        <v>-9.5950294852291118E-2</v>
-      </c>
-      <c r="F2" s="3">
-        <v>-0.98353428416386057</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="B2" s="2" t="n">
+        <v>-0.1014064422594133</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>-0.1014064422594133</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>-0.1946709524288406</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>-0.5209120364091356</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.66230799261827134</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.89896799999999999</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.50543531484681026</v>
-      </c>
-      <c r="E3" s="2">
-        <v>-0.18331408580421879</v>
-      </c>
-      <c r="F3" s="3">
-        <v>3.6129683636293102</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="B3" s="2" t="n">
+        <v>0.5614020711267445</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>0.4030658421573019</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>-0.2844594901863822</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>1.973574763699764</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.20080423435819639</v>
-      </c>
-      <c r="C4" s="2">
-        <v>-0.115118</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.80773310062041426</v>
-      </c>
-      <c r="E4" s="2">
-        <v>-0.1067686947478322</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1.880740743646427</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="B4" s="2" t="n">
+        <v>0.004154516839679934</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0.408894902825724</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>-0.1186527755524129</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0.03501407211367544</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2">
-        <v>-0.1158133288360743</v>
-      </c>
-      <c r="C5" s="2">
-        <v>-0.26458500000000001</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.59837351259040594</v>
-      </c>
-      <c r="E5" s="2">
-        <v>-0.1185678963155373</v>
-      </c>
-      <c r="F5" s="3">
-        <v>-0.97676801592116935</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="B5" s="2" t="n">
+        <v>-0.06168161780903469</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>0.3219919858965306</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>-0.06617199562095488</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>-0.9321408131977479</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2">
-        <v>-4.9622681053723687E-2</v>
-      </c>
-      <c r="C6" s="2">
-        <v>9.7531000000000007E-2</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.51905793357041219</v>
-      </c>
-      <c r="E6" s="2">
-        <v>-0.16980413372455769</v>
-      </c>
-      <c r="F6" s="3">
-        <v>-0.29223482353037128</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="B6" s="2" t="n">
+        <v>-0.03569604873815979</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0.2748020955365114</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>-0.1201466849840861</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>-0.2971039004770533</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2">
-        <v>7.8758544259091456E-2</v>
-      </c>
-      <c r="C7" s="2">
-        <v>-7.6999999999999999E-2</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.6386967250636415</v>
-      </c>
-      <c r="E7" s="2">
-        <v>-0.1060564755626895</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.74260948085661815</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="B7" s="2" t="n">
+        <v>0.09176833311728116</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0.3917885588983141</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>-0.06149243220476708</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>1.49235165738276</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.70856848515198689</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.52185199999999998</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.7998255811655079</v>
-      </c>
-      <c r="E8" s="2">
-        <v>-9.7996001765482732E-2</v>
-      </c>
-      <c r="F8" s="3">
-        <v>7.2305856605015792</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="B8" s="2" t="n">
+        <v>0.5668496493032291</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>1.18072341541407</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>-0.04475707222046588</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>12.66502970773026</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="2">
-        <v>0.56661153812513043</v>
-      </c>
-      <c r="C9" s="2">
-        <v>2.4566999999999999E-2</v>
-      </c>
-      <c r="D9" s="2">
-        <v>3.3862390601917838</v>
-      </c>
-      <c r="E9" s="2">
-        <v>-0.25223005241524282</v>
-      </c>
-      <c r="F9" s="3">
-        <v>2.2464077246129488</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="B9" s="2" t="n">
+        <v>0.2094109499002417</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>1.63739077730563</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>-0.1951849360569879</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>1.072884793932561</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="2">
-        <v>-3.0807631411380099E-2</v>
-      </c>
-      <c r="C10" s="2">
-        <v>-4.5830999999999997E-2</v>
-      </c>
-      <c r="D10" s="2">
-        <v>3.251109423943197</v>
-      </c>
-      <c r="E10" s="2">
-        <v>-7.6526739828513324E-2</v>
-      </c>
-      <c r="F10" s="3">
-        <v>-0.40257342048565092</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="B10" s="2" t="n">
+        <v>-0.03873749011555916</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>1.535224878138886</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>-0.05420362907940335</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>-0.7146659877480211</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="2">
-        <v>0.1663498280017639</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0.206036</v>
-      </c>
-      <c r="D11" s="2">
-        <v>3.9582807454328259</v>
-      </c>
-      <c r="E11" s="2">
-        <v>-5.2367316060368818E-2</v>
-      </c>
-      <c r="F11" s="3">
-        <v>3.176596406239276</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="B11" s="2" t="n">
+        <v>0.07367530923696508</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1.722008355021016</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>-0.01894768916755873</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>3.888353275454201</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="2">
-        <v>-5.5445588490634301E-2</v>
-      </c>
-      <c r="C12" s="2">
-        <v>-0.18013999999999999</v>
-      </c>
-      <c r="D12" s="2">
-        <v>3.6833659516005222</v>
-      </c>
-      <c r="E12" s="2">
-        <v>-9.8358294265828539E-2</v>
-      </c>
-      <c r="F12" s="3">
-        <v>-0.56371035004718573</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="B12" s="2" t="n">
+        <v>-0.03002707757057232</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>1.640274398997054</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>-0.04181430541017894</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>-0.7181053774783682</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:B12">
-    <cfRule type="dataBar" priority="2">
-      <dataBar maxLength="60">
+    <cfRule priority="1" type="dataBar">
+      <dataBar maxLength="60" showValue="1">
         <cfvo type="percentile" val="0"/>
         <cfvo type="percentile" val="99"/>
         <color rgb="FFFF0000"/>
       </dataBar>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E12">
-    <cfRule type="dataBar" priority="3">
-      <dataBar maxLength="60">
+  <conditionalFormatting sqref="D2:D12">
+    <cfRule priority="2" type="dataBar">
+      <dataBar maxLength="60" showValue="1">
         <cfvo type="percentile" val="90"/>
         <cfvo type="percentile" val="0"/>
-        <color rgb="FF22AE6B"/>
+        <color rgb="FF22ae6b"/>
       </dataBar>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C12">
-    <cfRule type="dataBar" priority="1">
-      <dataBar maxLength="60">
-        <cfvo type="percentile" val="0"/>
-        <cfvo type="percentile" val="99"/>
-        <color rgb="FFFF0000"/>
-      </dataBar>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>